<commit_message>
Fixed Book table and advanced queries
-Cleaned price data for Book and re-imported as new table (Price is now of type int instead of string)
-Added email attribute for Customer
-Updated advanced queries to work as expected (and with edited schema)
</commit_message>
<xml_diff>
--- a/Proj_Data_CSV.xlsx
+++ b/Proj_Data_CSV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\Documents\_UNIVERSITY\Schoolwork\DBSystems\Project\DBSysProj3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75153BF9-3B3D-41FF-87D2-00875B7262CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FC55FD-7B8C-4CE0-AFBC-5FB5C997DD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1741,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M100" sqref="M100"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,18 +1923,18 @@
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P4" t="s">
         <v>271</v>
       </c>
       <c r="R4">
         <f ca="1">RANDBETWEEN(1,20)</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="S4">
         <f ca="1">RANDBETWEEN(1,20)</f>
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -1983,11 +1983,11 @@
       </c>
       <c r="R5">
         <f t="shared" ref="R5:S18" ca="1" si="1">RANDBETWEEN(1,20)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="S5">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -2029,18 +2029,18 @@
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P6" t="s">
         <v>271</v>
       </c>
       <c r="R6">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="S6">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -2089,11 +2089,11 @@
       </c>
       <c r="R7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="S7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -2142,11 +2142,11 @@
       </c>
       <c r="R8">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="S8">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -2188,18 +2188,18 @@
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P9" t="s">
         <v>271</v>
       </c>
       <c r="R9">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="S9">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -2241,18 +2241,18 @@
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P10" t="s">
         <v>271</v>
       </c>
       <c r="R10">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="S10">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -2301,11 +2301,11 @@
       </c>
       <c r="R11">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S11">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -2347,18 +2347,18 @@
       </c>
       <c r="O12">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P12" t="s">
         <v>271</v>
       </c>
       <c r="R12">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S12">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="U12">
         <v>5</v>
@@ -2410,11 +2410,11 @@
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -2456,18 +2456,18 @@
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P14" t="s">
         <v>271</v>
       </c>
       <c r="R14">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="S14">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -2509,18 +2509,18 @@
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P15" t="s">
         <v>271</v>
       </c>
       <c r="R15">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="S15">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -2562,18 +2562,18 @@
       </c>
       <c r="O16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P16" t="s">
         <v>271</v>
       </c>
       <c r="R16">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -2619,11 +2619,11 @@
       </c>
       <c r="R17">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -2662,18 +2662,18 @@
       </c>
       <c r="O18">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P18" t="s">
         <v>271</v>
       </c>
       <c r="R18">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -2712,7 +2712,7 @@
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P19" t="s">
         <v>271</v>
@@ -2796,7 +2796,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P21" t="s">
         <v>271</v>
@@ -2838,7 +2838,7 @@
       </c>
       <c r="O22">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P22" t="s">
         <v>271</v>
@@ -2925,7 +2925,7 @@
       </c>
       <c r="O24">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P24" t="s">
         <v>271</v>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P26" t="s">
         <v>271</v>
@@ -3051,7 +3051,7 @@
       </c>
       <c r="O27">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P27" t="s">
         <v>271</v>
@@ -3093,7 +3093,7 @@
       </c>
       <c r="O28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P28" t="s">
         <v>271</v>
@@ -3135,7 +3135,7 @@
       </c>
       <c r="O29">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P29" t="s">
         <v>271</v>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="O32">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P32" t="s">
         <v>271</v>
@@ -3303,7 +3303,7 @@
       </c>
       <c r="O33">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P33" t="s">
         <v>271</v>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="O34">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P34" t="s">
         <v>271</v>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="O35">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P35" t="s">
         <v>271</v>
@@ -3429,7 +3429,7 @@
       </c>
       <c r="O36">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P36" t="s">
         <v>271</v>
@@ -3513,7 +3513,7 @@
       </c>
       <c r="O38">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P38" t="s">
         <v>271</v>
@@ -3555,7 +3555,7 @@
       </c>
       <c r="O39">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P39" t="s">
         <v>271</v>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="O40">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P40" t="s">
         <v>271</v>
@@ -3681,7 +3681,7 @@
       </c>
       <c r="O42">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P42" t="s">
         <v>271</v>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="O43">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P43" t="s">
         <v>271</v>
@@ -3807,7 +3807,7 @@
       </c>
       <c r="O45">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P45" t="s">
         <v>271</v>
@@ -3891,7 +3891,7 @@
       </c>
       <c r="O47">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P47" t="s">
         <v>271</v>
@@ -3933,7 +3933,7 @@
       </c>
       <c r="O48">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P48" t="s">
         <v>271</v>
@@ -4104,7 +4104,7 @@
       </c>
       <c r="O52">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P52" t="s">
         <v>271</v>
@@ -4146,7 +4146,7 @@
       </c>
       <c r="O53">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P53" t="s">
         <v>271</v>
@@ -4188,7 +4188,7 @@
       </c>
       <c r="O54">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P54" t="s">
         <v>271</v>
@@ -4230,7 +4230,7 @@
       </c>
       <c r="O55">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P55" t="s">
         <v>271</v>
@@ -4272,7 +4272,7 @@
       </c>
       <c r="O56">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P56" t="s">
         <v>271</v>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="O57">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P57" t="s">
         <v>271</v>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="O59">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P59" t="s">
         <v>271</v>
@@ -4527,7 +4527,7 @@
       </c>
       <c r="O62">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P62" t="s">
         <v>271</v>
@@ -4569,7 +4569,7 @@
       </c>
       <c r="O63">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P63" t="s">
         <v>271</v>
@@ -4611,7 +4611,7 @@
       </c>
       <c r="O64">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P64" t="s">
         <v>271</v>
@@ -4653,7 +4653,7 @@
       </c>
       <c r="O65">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P65" t="s">
         <v>271</v>
@@ -4695,7 +4695,7 @@
       </c>
       <c r="O66">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P66" t="s">
         <v>271</v>
@@ -4737,7 +4737,7 @@
       </c>
       <c r="O67">
         <f t="shared" ref="O67:O109" ca="1" si="2">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P67" t="s">
         <v>271</v>
@@ -4779,7 +4779,7 @@
       </c>
       <c r="O68">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P68" t="s">
         <v>271</v>
@@ -4821,7 +4821,7 @@
       </c>
       <c r="O69">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P69" t="s">
         <v>271</v>
@@ -5073,7 +5073,7 @@
       </c>
       <c r="O75">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P75" t="s">
         <v>271</v>
@@ -5157,7 +5157,7 @@
       </c>
       <c r="O77">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P77" t="s">
         <v>271</v>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="O78">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P78" t="s">
         <v>271</v>
@@ -5244,7 +5244,7 @@
       </c>
       <c r="O79">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P79" t="s">
         <v>271</v>
@@ -5286,7 +5286,7 @@
       </c>
       <c r="O80">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P80" t="s">
         <v>271</v>
@@ -5412,7 +5412,7 @@
       </c>
       <c r="O83">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P83" t="s">
         <v>271</v>
@@ -5454,7 +5454,7 @@
       </c>
       <c r="O84">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P84" t="s">
         <v>271</v>
@@ -5496,7 +5496,7 @@
       </c>
       <c r="O85">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P85" t="s">
         <v>271</v>
@@ -5580,7 +5580,7 @@
       </c>
       <c r="O87">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P87" t="s">
         <v>271</v>
@@ -5625,7 +5625,7 @@
       </c>
       <c r="O88">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P88" t="s">
         <v>271</v>
@@ -5667,7 +5667,7 @@
       </c>
       <c r="O89">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P89" t="s">
         <v>271</v>
@@ -5751,7 +5751,7 @@
       </c>
       <c r="O91">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P91" t="s">
         <v>271</v>
@@ -5793,7 +5793,7 @@
       </c>
       <c r="O92">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P92" t="s">
         <v>271</v>
@@ -5835,7 +5835,7 @@
       </c>
       <c r="O93">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P93" t="s">
         <v>271</v>
@@ -5877,7 +5877,7 @@
       </c>
       <c r="O94">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P94" t="s">
         <v>271</v>
@@ -5919,7 +5919,7 @@
       </c>
       <c r="O95">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P95" t="s">
         <v>271</v>
@@ -5964,7 +5964,7 @@
       </c>
       <c r="O96">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P96" t="s">
         <v>271</v>
@@ -6132,7 +6132,7 @@
       </c>
       <c r="O100">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P100" t="s">
         <v>271</v>
@@ -6261,7 +6261,7 @@
       </c>
       <c r="O103">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P103" t="s">
         <v>271</v>
@@ -6303,7 +6303,7 @@
       </c>
       <c r="O104">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P104" t="s">
         <v>271</v>
@@ -6345,7 +6345,7 @@
       </c>
       <c r="O105">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P105" t="s">
         <v>271</v>
@@ -6429,7 +6429,7 @@
       </c>
       <c r="O107">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P107" t="s">
         <v>271</v>
@@ -6471,7 +6471,7 @@
       </c>
       <c r="O108">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P108" t="s">
         <v>271</v>
@@ -6513,7 +6513,7 @@
       </c>
       <c r="O109">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P109" t="s">
         <v>271</v>
@@ -6524,6 +6524,99 @@
     <sortCondition ref="K2:K109"/>
   </sortState>
   <mergeCells count="108">
+    <mergeCell ref="H107:J107"/>
+    <mergeCell ref="H108:J108"/>
+    <mergeCell ref="H109:J109"/>
+    <mergeCell ref="H101:J101"/>
+    <mergeCell ref="H102:J102"/>
+    <mergeCell ref="H103:J103"/>
+    <mergeCell ref="H104:J104"/>
+    <mergeCell ref="H105:J105"/>
+    <mergeCell ref="H106:J106"/>
+    <mergeCell ref="H95:J95"/>
+    <mergeCell ref="H96:J96"/>
+    <mergeCell ref="H97:J97"/>
+    <mergeCell ref="H98:J98"/>
+    <mergeCell ref="H99:J99"/>
+    <mergeCell ref="H100:J100"/>
+    <mergeCell ref="H89:J89"/>
+    <mergeCell ref="H90:J90"/>
+    <mergeCell ref="H91:J91"/>
+    <mergeCell ref="H92:J92"/>
+    <mergeCell ref="H93:J93"/>
+    <mergeCell ref="H94:J94"/>
+    <mergeCell ref="H83:J83"/>
+    <mergeCell ref="H84:J84"/>
+    <mergeCell ref="H85:J85"/>
+    <mergeCell ref="H86:J86"/>
+    <mergeCell ref="H87:J87"/>
+    <mergeCell ref="H88:J88"/>
+    <mergeCell ref="H77:J77"/>
+    <mergeCell ref="H78:J78"/>
+    <mergeCell ref="H79:J79"/>
+    <mergeCell ref="H80:J80"/>
+    <mergeCell ref="H81:J81"/>
+    <mergeCell ref="H82:J82"/>
+    <mergeCell ref="H71:J71"/>
+    <mergeCell ref="H72:J72"/>
+    <mergeCell ref="H73:J73"/>
+    <mergeCell ref="H74:J74"/>
+    <mergeCell ref="H75:J75"/>
+    <mergeCell ref="H76:J76"/>
+    <mergeCell ref="H65:J65"/>
+    <mergeCell ref="H66:J66"/>
+    <mergeCell ref="H67:J67"/>
+    <mergeCell ref="H68:J68"/>
+    <mergeCell ref="H69:J69"/>
+    <mergeCell ref="H70:J70"/>
+    <mergeCell ref="H59:J59"/>
+    <mergeCell ref="H60:J60"/>
+    <mergeCell ref="H61:J61"/>
+    <mergeCell ref="H62:J62"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="H64:J64"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="H54:J54"/>
+    <mergeCell ref="H55:J55"/>
+    <mergeCell ref="H56:J56"/>
+    <mergeCell ref="H57:J57"/>
+    <mergeCell ref="H58:J58"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="H49:J49"/>
+    <mergeCell ref="H50:J50"/>
+    <mergeCell ref="H51:J51"/>
+    <mergeCell ref="H52:J52"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="H13:J13"/>
@@ -6539,99 +6632,6 @@
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="H49:J49"/>
-    <mergeCell ref="H50:J50"/>
-    <mergeCell ref="H51:J51"/>
-    <mergeCell ref="H52:J52"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="H59:J59"/>
-    <mergeCell ref="H60:J60"/>
-    <mergeCell ref="H61:J61"/>
-    <mergeCell ref="H62:J62"/>
-    <mergeCell ref="H63:J63"/>
-    <mergeCell ref="H64:J64"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="H54:J54"/>
-    <mergeCell ref="H55:J55"/>
-    <mergeCell ref="H56:J56"/>
-    <mergeCell ref="H57:J57"/>
-    <mergeCell ref="H58:J58"/>
-    <mergeCell ref="H71:J71"/>
-    <mergeCell ref="H72:J72"/>
-    <mergeCell ref="H73:J73"/>
-    <mergeCell ref="H74:J74"/>
-    <mergeCell ref="H75:J75"/>
-    <mergeCell ref="H76:J76"/>
-    <mergeCell ref="H65:J65"/>
-    <mergeCell ref="H66:J66"/>
-    <mergeCell ref="H67:J67"/>
-    <mergeCell ref="H68:J68"/>
-    <mergeCell ref="H69:J69"/>
-    <mergeCell ref="H70:J70"/>
-    <mergeCell ref="H83:J83"/>
-    <mergeCell ref="H84:J84"/>
-    <mergeCell ref="H85:J85"/>
-    <mergeCell ref="H86:J86"/>
-    <mergeCell ref="H87:J87"/>
-    <mergeCell ref="H88:J88"/>
-    <mergeCell ref="H77:J77"/>
-    <mergeCell ref="H78:J78"/>
-    <mergeCell ref="H79:J79"/>
-    <mergeCell ref="H80:J80"/>
-    <mergeCell ref="H81:J81"/>
-    <mergeCell ref="H82:J82"/>
-    <mergeCell ref="H95:J95"/>
-    <mergeCell ref="H96:J96"/>
-    <mergeCell ref="H97:J97"/>
-    <mergeCell ref="H98:J98"/>
-    <mergeCell ref="H99:J99"/>
-    <mergeCell ref="H100:J100"/>
-    <mergeCell ref="H89:J89"/>
-    <mergeCell ref="H90:J90"/>
-    <mergeCell ref="H91:J91"/>
-    <mergeCell ref="H92:J92"/>
-    <mergeCell ref="H93:J93"/>
-    <mergeCell ref="H94:J94"/>
-    <mergeCell ref="H107:J107"/>
-    <mergeCell ref="H108:J108"/>
-    <mergeCell ref="H109:J109"/>
-    <mergeCell ref="H101:J101"/>
-    <mergeCell ref="H102:J102"/>
-    <mergeCell ref="H103:J103"/>
-    <mergeCell ref="H104:J104"/>
-    <mergeCell ref="H105:J105"/>
-    <mergeCell ref="H106:J106"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>

</xml_diff>